<commit_message>
func to get data from col as relates to series
</commit_message>
<xml_diff>
--- a/twitter_analytics.xlsx
+++ b/twitter_analytics.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rachl\coding projects\metrospeedy-social-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8B2A3DE8-426A-4F9B-AF70-318B5BE40E81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A17B246-C82B-4B51-A808-10CFDBE06ADB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="twitter_analytics" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -597,10 +597,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -628,10 +629,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -650,117 +652,6 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>twitter_analytics!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>impressions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent3">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>twitter_analytics!$A$2:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.81527777777777777</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.81180555555555556</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.69444444444444453</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.84375</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.8881944444444444</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.3888888888888888E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>twitter_analytics!$B$2:$B$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>117</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>164</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1169</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1013</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1323</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-AB2A-47CB-A027-212D74877F68}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="3"/>
           <c:order val="1"/>
           <c:tx>
@@ -777,37 +668,23 @@
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
+              <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent4">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="3"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
               </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
+              <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -888,37 +765,23 @@
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
+              <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent1">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="3"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln>
-                <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
               </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
+              <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -996,21 +859,21 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
               <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="3"/>
+                <c:idx val="2"/>
+                <c:order val="0"/>
                 <c:tx>
                   <c:strRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>twitter_analytics!$C$1</c15:sqref>
+                          <c15:sqref>twitter_analytics!$B$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>engagements</c:v>
+                        <c:v>impressions</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1018,37 +881,23 @@
                 <c:spPr>
                   <a:ln w="25400" cap="rnd">
                     <a:noFill/>
+                    <a:round/>
                   </a:ln>
-                  <a:effectLst>
-                    <a:glow rad="139700">
-                      <a:schemeClr val="accent2">
-                        <a:satMod val="175000"/>
-                        <a:alpha val="14000"/>
-                      </a:schemeClr>
-                    </a:glow>
-                  </a:effectLst>
+                  <a:effectLst/>
                 </c:spPr>
                 <c:marker>
                   <c:symbol val="circle"/>
-                  <c:size val="3"/>
+                  <c:size val="5"/>
                   <c:spPr>
                     <a:solidFill>
-                      <a:schemeClr val="accent2">
-                        <a:lumMod val="60000"/>
-                        <a:lumOff val="40000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="accent3"/>
                     </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
                     </a:ln>
-                    <a:effectLst>
-                      <a:glow rad="63500">
-                        <a:schemeClr val="accent2">
-                          <a:satMod val="175000"/>
-                          <a:alpha val="25000"/>
-                        </a:schemeClr>
-                      </a:glow>
-                    </a:effectLst>
+                    <a:effectLst/>
                   </c:spPr>
                 </c:marker>
                 <c:xVal>
@@ -1089,6 +938,123 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
+                          <c15:sqref>twitter_analytics!$B$2:$B$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>138</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>117</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>164</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1169</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1013</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1323</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000007-AB2A-47CB-A027-212D74877F68}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>twitter_analytics!$C$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>engagements</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>twitter_analytics!$A$2:$A$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>h:mm</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>0.81527777777777777</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.81180555555555556</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.69444444444444453</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.84375</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.8881944444444444</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.3888888888888888E-2</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
                           <c15:sqref>twitter_analytics!$C$2:$C$7</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
@@ -1118,7 +1084,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-AB2A-47CB-A027-212D74877F68}"/>
                   </c:ext>
@@ -1139,10 +1105,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1157,10 +1122,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1170,13 +1136,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>time</a:t>
+                  <a:t>time (military)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (military)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1193,10 +1154,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1215,7 +1177,12 @@
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
             <a:round/>
           </a:ln>
           <a:effectLst/>
@@ -1227,8 +1194,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1254,10 +1222,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1272,10 +1239,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1285,11 +1253,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>impressions/engagements</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> count</a:t>
+                  <a:t>impressions/engagements count</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1307,10 +1271,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1330,8 +1295,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1345,8 +1311,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1370,7 +1337,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1386,8 +1353,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="75000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1406,14 +1374,11 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="dk1">
+        <a:schemeClr val="tx1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1468,19 +1433,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -1800,7 +1759,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>twitter_analytics!$C$1</c15:sqref>
@@ -1875,7 +1834,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>twitter_analytics!$A$2:$A$7</c15:sqref>
@@ -1908,7 +1867,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>twitter_analytics!$C$2:$C$7</c15:sqref>
@@ -1940,7 +1899,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-49FE-4202-86FE-9E238E7341FD}"/>
                   </c:ext>
@@ -1961,9 +1920,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1978,10 +1937,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1991,11 +1951,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>time</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (military)</a:t>
+                  <a:t>time (military)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2013,10 +1969,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -2034,12 +1991,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2050,8 +2003,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -2077,9 +2031,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -2094,10 +2048,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -2107,13 +2062,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>engagement</a:t>
+                  <a:t>engagement rate</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> rate</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2130,10 +2080,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -2151,12 +2102,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2167,8 +2114,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -2208,8 +2156,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="75000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -2233,28 +2182,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -2354,35 +2292,211 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2393,7 +2507,357 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2408,560 +2872,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="15000"/>
-        <a:lumOff val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="139700">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="14000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:lumMod val="60000"/>
-          <a:lumOff val="40000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-            <a:alpha val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2980,6 +2893,14 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -3068,18 +2989,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3089,20 +3013,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3116,14 +3040,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -3137,8 +3061,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3150,7 +3075,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -3163,9 +3088,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3180,13 +3105,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -3198,14 +3124,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -3217,13 +3143,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -3232,8 +3159,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3243,7 +3171,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D>
@@ -3251,7 +3179,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -3259,17 +3187,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3279,14 +3210,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3298,19 +3229,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -3319,14 +3243,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -3335,8 +3258,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3346,7 +3270,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -3354,9 +3278,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3367,19 +3291,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -3387,7 +3303,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -3440,9 +3356,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
+      <xdr:colOff>594360</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3766,11 +3682,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>